<commit_message>
[WIP] wifi checklist backend
</commit_message>
<xml_diff>
--- a/Db_structure/DB_structure.xlsx
+++ b/Db_structure/DB_structure.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\checklist-system\Db_structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3008D8-18B2-4B4E-9AB4-4C35F2762772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,20 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
-  <si>
-    <t>wifi_index</t>
-  </si>
-  <si>
-    <t>tb_wifi</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
   <si>
     <t>wifi_name</t>
   </si>
   <si>
-    <t>tb_checklist_wifi</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -47,9 +39,6 @@
     <t>check_date</t>
   </si>
   <si>
-    <t>chk_index</t>
-  </si>
-  <si>
     <t>check_time</t>
   </si>
   <si>
@@ -99,17 +88,161 @@
   </si>
   <si>
     <t>lan_wire</t>
+  </si>
+  <si>
+    <t>User or Member</t>
+  </si>
+  <si>
+    <t>tbl_user</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>user_code</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>dept_id</t>
+  </si>
+  <si>
+    <t>position_id</t>
+  </si>
+  <si>
+    <t>user_status</t>
+  </si>
+  <si>
+    <t>int(11)</t>
+  </si>
+  <si>
+    <t>tbl_list_wifi</t>
+  </si>
+  <si>
+    <t>tbl_checklist_wifi</t>
+  </si>
+  <si>
+    <t>tbl_repair_wifi</t>
+  </si>
+  <si>
+    <t>rp_id</t>
+  </si>
+  <si>
+    <t>wifi_id</t>
+  </si>
+  <si>
+    <t>chk_id</t>
+  </si>
+  <si>
+    <t>rp_status</t>
+  </si>
+  <si>
+    <t>rp_date</t>
+  </si>
+  <si>
+    <t>rp_comments</t>
+  </si>
+  <si>
+    <t>int(defalut(0))</t>
+  </si>
+  <si>
+    <t>int(default(null))</t>
+  </si>
+  <si>
+    <t>tbl_equipment_status</t>
+  </si>
+  <si>
+    <t>eqs_id</t>
+  </si>
+  <si>
+    <t>eqs_name</t>
+  </si>
+  <si>
+    <t>Equipment status</t>
+  </si>
+  <si>
+    <t>wifi_index,</t>
+  </si>
+  <si>
+    <t>check_date,</t>
+  </si>
+  <si>
+    <t>check_time,</t>
+  </si>
+  <si>
+    <t>re_time,</t>
+  </si>
+  <si>
+    <t>up_time,</t>
+  </si>
+  <si>
+    <t>check_ping,</t>
+  </si>
+  <si>
+    <t>led_lan,</t>
+  </si>
+  <si>
+    <t>led_24g,</t>
+  </si>
+  <si>
+    <t>led_5g,</t>
+  </si>
+  <si>
+    <t>led_power,</t>
+  </si>
+  <si>
+    <t>lan_wire,</t>
+  </si>
+  <si>
+    <t>wifi_dust,</t>
+  </si>
+  <si>
+    <t>mc_status,</t>
+  </si>
+  <si>
+    <t>rp_status,</t>
+  </si>
+  <si>
+    <t>remark,</t>
+  </si>
+  <si>
+    <t>user_id,</t>
+  </si>
+  <si>
+    <t>'17-5-2022',</t>
+  </si>
+  <si>
+    <t>'16:34:00',</t>
+  </si>
+  <si>
+    <t>'06:00:00',</t>
+  </si>
+  <si>
+    <t>'9H:34M',</t>
+  </si>
+  <si>
+    <t>yes'</t>
+  </si>
+  <si>
+    <t>1',</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -118,20 +251,42 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -274,11 +429,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -286,22 +524,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,208 +886,510 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.375" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.75" customWidth="1"/>
-    <col min="17" max="17" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7265625" customWidth="1"/>
+    <col min="17" max="17" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:22" ht="24" thickBot="1">
+      <c r="A1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="K1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="20"/>
+    </row>
+    <row r="2" spans="1:22" ht="15" thickBot="1">
+      <c r="A2" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
+      <c r="K2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15" thickBot="1">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="24" thickBot="1">
+      <c r="A5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="D6" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="28"/>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="V7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    </row>
+    <row r="8" spans="1:22" ht="15" thickBot="1">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="13"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="F8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15" thickBot="1"/>
+    <row r="10" spans="1:22" ht="15" thickBot="1">
+      <c r="A10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15" thickBot="1">
+      <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="B12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="H15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="H16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9">
+      <c r="H17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9">
+      <c r="H18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="8:9">
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="8:9">
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9">
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="8:9">
+      <c r="H22" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="8:9">
+      <c r="H23" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9">
+      <c r="H24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="8:9">
+      <c r="H25" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="8:9">
+      <c r="H26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="8:9">
+      <c r="H27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I27" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="8:9">
+      <c r="H28" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="8:9">
+      <c r="H29" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="U3" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>4</v>
+      <c r="I29" s="29" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="D2:R2"/>
+  <mergeCells count="8">
+    <mergeCell ref="D6:V6"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:S5"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add form id function
</commit_message>
<xml_diff>
--- a/Db_structure/DB_structure.xlsx
+++ b/Db_structure/DB_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\checklist-system\Db_structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66C0750-0C39-4C54-B66E-70E26C2602CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B057C6-9EEE-46C3-BF1B-CBB76637636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28690" yWindow="2890" windowWidth="20710" windowHeight="11740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
   <si>
     <t>wifi_name</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>tbl_auto_number</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>varchar(225)</t>
+  </si>
+  <si>
+    <t>ชื่อของอุปกร์</t>
   </si>
 </sst>
 </file>
@@ -504,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -529,18 +538,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -566,6 +563,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -884,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -894,7 +900,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.81640625" customWidth="1"/>
     <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.1796875" customWidth="1"/>
     <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
@@ -902,10 +908,10 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.54296875" bestFit="1" customWidth="1"/>
@@ -915,48 +921,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24" thickBot="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="K1" s="22" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="K1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="22"/>
-      <c r="N1" s="16" t="s">
+      <c r="L1" s="18"/>
+      <c r="N1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
-      <c r="K2" s="20" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+      <c r="K2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="21"/>
-      <c r="N2" s="17" t="s">
+      <c r="L2" s="17"/>
+      <c r="N2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="18"/>
-      <c r="P2" s="19"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27"/>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="2" t="s">
@@ -996,9 +1004,12 @@
         <v>64</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1040,9 +1051,12 @@
         <v>47</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1084,9 +1098,12 @@
         <v>57</v>
       </c>
       <c r="O5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1118,10 +1135,10 @@
       <c r="W8" s="15"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="24"/>
       <c r="D9" s="12" t="s">
         <v>32</v>
       </c>
@@ -1401,14 +1418,14 @@
   <mergeCells count="10">
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A8:W8"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D9:W9"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add checklist number generating function
</commit_message>
<xml_diff>
--- a/Db_structure/DB_structure.xlsx
+++ b/Db_structure/DB_structure.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\checklist-system\Db_structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B057C6-9EEE-46C3-BF1B-CBB76637636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="2890" windowWidth="20710" windowHeight="11740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="2895" windowWidth="20715" windowHeight="11745"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,12 +254,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -269,7 +268,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -277,7 +276,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -285,7 +284,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -887,40 +886,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6328125" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" customWidth="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.75" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="24" thickBot="1">
+    <row r="1" spans="1:23" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>20</v>
       </c>
@@ -943,7 +942,7 @@
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>21</v>
       </c>
@@ -966,7 +965,7 @@
       <c r="P2" s="26"/>
       <c r="Q2" s="27"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1013,7 +1012,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1060,7 +1059,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" thickBot="1">
+    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="24" thickBot="1">
+    <row r="8" spans="1:23" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
@@ -1134,7 +1133,7 @@
       <c r="V8" s="15"/>
       <c r="W8" s="15"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>31</v>
       </c>
@@ -1162,7 +1161,7 @@
       <c r="V9" s="13"/>
       <c r="W9" s="14"/>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1230,7 +1229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -1298,7 +1297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15" thickBot="1">
+    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>57</v>
       </c>
@@ -1328,10 +1327,10 @@
       <c r="V12" s="5"/>
       <c r="W12" s="6"/>
     </row>
-    <row r="13" spans="1:23" ht="15" thickBot="1">
+    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>33</v>
       </c>
@@ -1340,7 +1339,7 @@
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>34</v>
       </c>
@@ -1357,7 +1356,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1374,44 +1373,44 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1">
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I29" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[WIP] wifi check history
</commit_message>
<xml_diff>
--- a/Db_structure/DB_structure.xlsx
+++ b/Db_structure/DB_structure.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\checklist-system\Db_structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEBD3E2-F4EF-41DB-B111-B16962805A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="2895" windowWidth="20715" windowHeight="11745"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
   <si>
     <t>wifi_name</t>
   </si>
@@ -254,12 +255,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -268,7 +269,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -276,7 +277,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -284,7 +285,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -886,40 +887,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.125" customWidth="1"/>
-    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6328125" customWidth="1"/>
+    <col min="21" max="21" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="24" thickBot="1">
       <c r="A1" s="22" t="s">
         <v>20</v>
       </c>
@@ -942,7 +944,7 @@
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" s="19" t="s">
         <v>21</v>
       </c>
@@ -965,7 +967,7 @@
       <c r="P2" s="26"/>
       <c r="Q2" s="27"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1012,7 +1014,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1059,7 +1061,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
@@ -1106,7 +1108,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="24" thickBot="1">
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
@@ -1132,8 +1134,9 @@
       <c r="U8" s="15"/>
       <c r="V8" s="15"/>
       <c r="W8" s="15"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X8" s="15"/>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" s="23" t="s">
         <v>31</v>
       </c>
@@ -1159,9 +1162,10 @@
       <c r="T9" s="13"/>
       <c r="U9" s="13"/>
       <c r="V9" s="13"/>
-      <c r="W9" s="14"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W9" s="13"/>
+      <c r="X9" s="14"/>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1217,19 +1221,22 @@
         <v>37</v>
       </c>
       <c r="T10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U10" s="7" t="s">
+      <c r="V10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="V10" s="7" t="s">
+      <c r="W10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="W10" s="8" t="s">
+      <c r="X10" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -1288,16 +1295,19 @@
         <v>4</v>
       </c>
       <c r="U11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W11" s="3" t="s">
+      <c r="X11" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="15" thickBot="1">
       <c r="A12" s="4" t="s">
         <v>57</v>
       </c>
@@ -1325,12 +1335,13 @@
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
-      <c r="W12" s="6"/>
-    </row>
-    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W12" s="5"/>
+      <c r="X12" s="6"/>
+    </row>
+    <row r="13" spans="1:24" ht="15" thickBot="1">
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24">
       <c r="A14" s="12" t="s">
         <v>33</v>
       </c>
@@ -1339,7 +1350,7 @@
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24">
       <c r="A15" s="11" t="s">
         <v>34</v>
       </c>
@@ -1356,7 +1367,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1373,56 +1384,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" thickBot="1">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="I29" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A8:W8"/>
+    <mergeCell ref="A8:X8"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:W9"/>
+    <mergeCell ref="D9:X9"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="N1:Q1"/>
   </mergeCells>

</xml_diff>